<commit_message>
Add form for training pack.
</commit_message>
<xml_diff>
--- a/LF/TAS/Training Evaluation/test_tas.xlsx
+++ b/LF/TAS/Training Evaluation/test_tas.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\LF\TAS\Training Evaluation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbandubad\OneDrive - World Health Organization\Documents\Repositories\dsa-forms\LF\TAS\Training Evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA28ED18-AC8C-41F6-A1F9-6E1A92A4B743}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15360"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="121">
   <si>
     <t>type</t>
   </si>
@@ -231,9 +230,6 @@
     <t>list_ecole</t>
   </si>
   <si>
-    <t>media::image</t>
-  </si>
-  <si>
     <t>appearance</t>
   </si>
   <si>
@@ -363,12 +359,6 @@
     <t>q17</t>
   </si>
   <si>
-    <t>start</t>
-  </si>
-  <si>
-    <t>end</t>
-  </si>
-  <si>
     <t>label::French</t>
   </si>
   <si>
@@ -382,12 +372,24 @@
   </si>
   <si>
     <t>tas_test1</t>
+  </si>
+  <si>
+    <t>tel</t>
+  </si>
+  <si>
+    <t>Numéro de téléhone</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -895,14 +897,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -923,16 +925,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F1" s="29" t="s">
-        <v>69</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="13" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -947,7 +949,7 @@
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.2">
@@ -1030,7 +1032,7 @@
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="20" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -1080,7 +1082,7 @@
       </c>
       <c r="D13" s="22"/>
       <c r="E13" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.2">
@@ -1154,7 +1156,7 @@
       </c>
       <c r="D19" s="26"/>
       <c r="E19" s="31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="28" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
@@ -1233,7 +1235,7 @@
     </row>
     <row r="26" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B26" s="15" t="s">
         <v>57</v>
@@ -1247,13 +1249,13 @@
     </row>
     <row r="27" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B27" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="15" t="s">
         <v>83</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>84</v>
       </c>
       <c r="D27" s="15"/>
       <c r="E27" s="16"/>
@@ -1263,10 +1265,10 @@
         <v>3</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C28" s="33" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D28" s="16"/>
       <c r="E28" s="16"/>
@@ -1276,10 +1278,10 @@
         <v>43</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D29" s="16"/>
       <c r="E29" s="16"/>
@@ -1289,10 +1291,10 @@
         <v>3</v>
       </c>
       <c r="B30" s="34" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
@@ -1300,10 +1302,10 @@
         <v>3</v>
       </c>
       <c r="B31" s="34" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
@@ -1311,37 +1313,35 @@
         <v>3</v>
       </c>
       <c r="B32" s="34" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A33" s="15" t="s">
         <v>29</v>
       </c>
       <c r="B33" s="34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="34" t="s">
-        <v>113</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="15" t="s">
+        <v>2</v>
       </c>
       <c r="B34" s="34" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="34" t="s">
-        <v>114</v>
-      </c>
-      <c r="B35" s="34" t="s">
-        <v>114</v>
+        <v>117</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1356,7 +1356,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -1381,7 +1381,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1411,7 +1411,7 @@
         <v>68</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>58</v>
@@ -1422,7 +1422,7 @@
         <v>68</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>59</v>
@@ -1433,7 +1433,7 @@
         <v>68</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>60</v>
@@ -1444,7 +1444,7 @@
         <v>68</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>61</v>
@@ -1455,7 +1455,7 @@
         <v>68</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>62</v>
@@ -1466,7 +1466,7 @@
         <v>68</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>63</v>
@@ -1477,7 +1477,7 @@
         <v>68</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>64</v>
@@ -1488,7 +1488,7 @@
         <v>68</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>65</v>
@@ -1499,7 +1499,7 @@
         <v>68</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>66</v>
@@ -1510,7 +1510,7 @@
         <v>68</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>67</v>
@@ -1518,79 +1518,79 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -1872,7 +1872,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -1906,16 +1906,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C2">
         <v>200220</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E2" s="3"/>
     </row>

</xml_diff>